<commit_message>
se modifica excel y se terminan de agregar comentarios
</commit_message>
<xml_diff>
--- a/resultados/Soluciones Mochila Paso 3.xlsx
+++ b/resultados/Soluciones Mochila Paso 3.xlsx
@@ -96,12 +96,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -505,70 +506,70 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>[True, False, True]</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="n">
+          <t>Se almacenan los objetos: 1, 3</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="n">
         <v>132</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>[True, True, False]</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="n">
+          <t>Se almacenan los objetos: 1, 2</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="n">
         <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>[False, True, True]</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="n">
+          <t>Se almacenan los objetos: 2, 3</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
         <v>96</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>[True, False, False]</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n">
+          <t>Se almacena el objeto: 1</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n">
         <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>[False, False, True]</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="n">
+          <t>Se almacena el objeto: 3</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>[False, True, False]</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="n">
+          <t>Se almacena el objeto: 2</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>[False, False, False]</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="n">
+          <t>No se almacenan objetos</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>